<commit_message>
Redmine #9281 cal sheets added to repo for CP05MOAS added/updated for gliders 376, 379, 380, 387 for multiple deployments.
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL379/Omaha_Cal_Info_CP05MOAS-GL379_00001.xlsx
+++ b/CP05MOAS-GL379/Omaha_Cal_Info_CP05MOAS-GL379_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377"/>
+    <workbookView xWindow="680" yWindow="660" windowWidth="23180" windowHeight="7920" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,17 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$78</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$350</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Ref Des</t>
   </si>
@@ -97,12 +102,6 @@
     <t>CC_depolarization_ratio</t>
   </si>
   <si>
-    <t>39°57.693'N</t>
-  </si>
-  <si>
-    <t>70°54.483'W</t>
-  </si>
-  <si>
     <t>KN-217</t>
   </si>
   <si>
@@ -134,13 +133,22 @@
   </si>
   <si>
     <t>CP05MOAS-GL379</t>
+  </si>
+  <si>
+    <t>39° 50' N</t>
+  </si>
+  <si>
+    <t>70° 42.5' W</t>
+  </si>
+  <si>
+    <t>FZ-1 Line</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -217,12 +225,17 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,12 +246,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCECFF"/>
         <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -312,14 +319,14 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="hair">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="hair">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -351,13 +358,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -379,9 +380,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,14 +387,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="8" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -774,26 +781,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="39.42578125"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125"/>
-    <col min="7" max="7" width="18.7109375"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="51.7109375"/>
-    <col min="12" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,10 +805,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -828,50 +829,57 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:13" s="8" customFormat="1" ht="15">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="9">
+        <v>379</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24">
+        <v>41750</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="F2" s="24">
+        <v>41831</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10">
-        <v>379</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11">
-        <v>41744</v>
-      </c>
-      <c r="E2" s="12">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="F2" s="25">
-        <v>41918</v>
-      </c>
-      <c r="G2" s="21" t="s">
+      <c r="I2" s="27">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="10">
-        <v>0</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="23">
+      <c r="K2" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="20">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>39.961550000000003</v>
-      </c>
-      <c r="M2" s="23">
+        <v>39.833333333333336</v>
+      </c>
+      <c r="M2" s="20">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.908050000000003</v>
+        <v>-70.708333333333329</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -879,29 +887,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875"/>
-    <col min="8" max="8" width="14.42578125"/>
-    <col min="9" max="9" width="13.42578125"/>
-    <col min="10" max="1024" width="8.7109375"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
@@ -916,377 +920,382 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="14">
+        <v>379</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18">
+        <v>649982</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="14">
+        <v>379</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18">
+        <v>649982</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14">
+        <v>379</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
+        <v>649982</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14">
+        <v>379</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>649982</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" s="6" customFormat="1">
+      <c r="A7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="14">
+        <v>379</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18">
+        <v>3116</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="23">
+        <v>124</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" s="6" customFormat="1">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="14">
+        <v>379</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18">
+        <v>3116</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="22">
+        <v>700</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:15" s="6" customFormat="1">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="14">
+        <v>379</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
+        <v>3116</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="23">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" s="6" customFormat="1">
+      <c r="A10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="14">
+        <v>379</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <v>3116</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="22">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:15" s="6" customFormat="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:15" s="6" customFormat="1">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B12" s="14">
         <v>379</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="20">
-        <v>649982</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="24">
-        <v>0.61</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="16">
+      <c r="D12" s="18">
+        <v>9057</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:15" s="6" customFormat="1">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:15" s="6" customFormat="1">
+      <c r="A14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="14">
         <v>379</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C14" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="20">
-        <v>649982</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="24">
-        <v>0.61</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="D14" s="18">
+        <v>178</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:15" s="6" customFormat="1">
+      <c r="A15" s="11"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:15" s="6" customFormat="1">
+      <c r="A16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="14">
         <v>379</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C16" s="14">
         <v>1</v>
       </c>
-      <c r="D4" s="20">
-        <v>649982</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.61</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="D16" s="18">
+        <v>50158</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" s="6" customFormat="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" s="6" customFormat="1">
+      <c r="A18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="14">
         <v>379</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C18" s="14">
         <v>1</v>
       </c>
-      <c r="D5" s="20">
-        <v>649982</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="24">
-        <v>0.61</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="D18" s="25">
         <v>379</v>
       </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="20">
-        <v>3116</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="27">
-        <v>124</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="16">
-        <v>379</v>
-      </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20">
-        <v>3116</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="26">
-        <v>700</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="16">
-        <v>379</v>
-      </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="20">
-        <v>3116</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="27">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="16">
-        <v>379</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20">
-        <v>3116</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="26">
-        <v>3.9E-2</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="16">
-        <v>379</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="20">
-        <v>9057</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="16">
-        <v>379</v>
-      </c>
-      <c r="C14" s="16">
-        <v>1</v>
-      </c>
-      <c r="D14" s="20">
-        <v>178</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="16">
-        <v>379</v>
-      </c>
-      <c r="C16" s="16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20">
-        <v>50158</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="16">
-        <v>379</v>
-      </c>
-      <c r="C18" s="16">
-        <v>1</v>
-      </c>
-      <c r="D18" s="20">
-        <v>374</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" s="6" customFormat="1">
+      <c r="A19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>